<commit_message>
Correspondence and Consultant Advice are marked for executed (only for Demo)
</commit_message>
<xml_diff>
--- a/Falcrum_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
+++ b/Falcrum_Trunk/src/com/proj/suite/TRANSMITTALS Suite.xlsx
@@ -498,7 +498,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -577,7 +577,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">

</xml_diff>